<commit_message>
added flex box to flexboxstyle.css
</commit_message>
<xml_diff>
--- a/It's 5 o'clock somewhere .xlsx
+++ b/It's 5 o'clock somewhere .xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14640" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14600" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Current Code" sheetId="3" r:id="rId1"/>
@@ -2075,7 +2075,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -3188,7 +3187,6 @@
     <hyperlink ref="G13" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>